<commit_message>
Header page manual test cases
</commit_message>
<xml_diff>
--- a/LumaProject/TestCases/Test Cases.xlsx
+++ b/LumaProject/TestCases/Test Cases.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW Testing\Automation Projects\LumaProject\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1AE973-CCCF-45E7-A054-958CFB9B6D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8386813-51AF-441C-AF2A-87BDDFC15055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="HeaderPage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="86">
   <si>
     <t xml:space="preserve">Expected Results </t>
   </si>
@@ -37,9 +37,6 @@
     <t>Steps</t>
   </si>
   <si>
-    <t xml:space="preserve">Assgine </t>
-  </si>
-  <si>
     <t>Req. ID</t>
   </si>
   <si>
@@ -92,6 +89,201 @@
   </si>
   <si>
     <t>Edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify visibility of Luma logo </t>
+  </si>
+  <si>
+    <t>Open any page</t>
+  </si>
+  <si>
+    <t>Luma logo is visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify visibility of what's new button </t>
+  </si>
+  <si>
+    <t>What's new button  is visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify visibility of women button </t>
+  </si>
+  <si>
+    <t>Women button  is visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify visibility of men button </t>
+  </si>
+  <si>
+    <t>Men button  is visible</t>
+  </si>
+  <si>
+    <t>Verify visibility of gear button</t>
+  </si>
+  <si>
+    <t>Gear button  is visible</t>
+  </si>
+  <si>
+    <t>Verify visibility of training button</t>
+  </si>
+  <si>
+    <t>Training button  is visible</t>
+  </si>
+  <si>
+    <t>Verify visibility of sale button</t>
+  </si>
+  <si>
+    <t>Sale button  is visible</t>
+  </si>
+  <si>
+    <t>Verify visibility of sign in button</t>
+  </si>
+  <si>
+    <t>Sign in button  is visible</t>
+  </si>
+  <si>
+    <t>Verify visibility of create an account button</t>
+  </si>
+  <si>
+    <t>Create an account button  is visible</t>
+  </si>
+  <si>
+    <t>Verify visibility of search bar</t>
+  </si>
+  <si>
+    <t>Search bar is visible</t>
+  </si>
+  <si>
+    <t>Verify visibility of cart button</t>
+  </si>
+  <si>
+    <t>Cart button is visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify functionality of Luma logo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on Luma logo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to home page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify functionality of what's new button </t>
+  </si>
+  <si>
+    <t>Click on what's new button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to what's new page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify functionality of  women button </t>
+  </si>
+  <si>
+    <t>Click on women button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to women page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify functionality of  men button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on men button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to men page </t>
+  </si>
+  <si>
+    <t>Verify functionality of gear button</t>
+  </si>
+  <si>
+    <t>Click on gear button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to gear page </t>
+  </si>
+  <si>
+    <t>Verify functionality of training button</t>
+  </si>
+  <si>
+    <t>Click on training button</t>
+  </si>
+  <si>
+    <t>Verify functionality of sale button</t>
+  </si>
+  <si>
+    <t>Click on sale button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to sale page </t>
+  </si>
+  <si>
+    <t>Verify functionality of sign in button</t>
+  </si>
+  <si>
+    <t>Click on sign in button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to sign in page </t>
+  </si>
+  <si>
+    <t>Verify functionality of create an account button</t>
+  </si>
+  <si>
+    <t>Click on create an account button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to create an account page </t>
+  </si>
+  <si>
+    <t>Verify functionality of cart button</t>
+  </si>
+  <si>
+    <t>Click on cart button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to cart page </t>
+  </si>
+  <si>
+    <t>Verify functionality of search bard</t>
+  </si>
+  <si>
+    <t>Click on search icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to search result page </t>
+  </si>
+  <si>
+    <t>Enter data less than the minimum search query (less than 3 char)</t>
+  </si>
+  <si>
+    <t>An error message appears that says "Minimum Search query length is 3"</t>
+  </si>
+  <si>
+    <t>Verify leaving search field empty</t>
+  </si>
+  <si>
+    <t>User stays in the same page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is navigated to training page </t>
+  </si>
+  <si>
+    <t>Enter valid search data</t>
+  </si>
+  <si>
+    <t>Search data is entered correctly</t>
+  </si>
+  <si>
+    <t>Verify entering search data less than minimum search query</t>
+  </si>
+  <si>
+    <t>Leave search field empty and click on search icon</t>
   </si>
 </sst>
 </file>
@@ -540,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F03D4B-6804-4012-A9F1-1BCB63C138AF}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -553,15 +745,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="10">
         <v>45778</v>
@@ -569,50 +761,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -622,17 +814,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130E7D9E-6773-4033-B48B-95B5E50BE331}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -653,24 +845,24 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -685,7 +877,9 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="3"/>
       <c r="E3" s="7"/>
@@ -698,25 +892,1172 @@
       <c r="A4" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>12.1</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>13</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>13.1</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>13.2</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>14</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>15</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>15.1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>15.2</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>16</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>16.2</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>17</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>17.2</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>18</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>18.2</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>19</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>20</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>20.2</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>21</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>22</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="5"/>
+      <c r="E56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
+        <v>23</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C59" s="7"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
+        <v>23.1</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
+        <v>24</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="4">
+        <v>24.1</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="4">
+        <v>24.2</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{8D60AC27-E235-47B3-9C43-1F9D9C6BDE3E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G6 G8 G10 G12 G14 G16 G18 G20 G22 G24 G26:G27 G29:G30 G32:G33 G35:G36 G38:G39 G41:G42 G44:G45 G47:G48 G50:G51 G53:G54 G56:G58 G60:G62 G64:G65" xr:uid="{8D60AC27-E235-47B3-9C43-1F9D9C6BDE3E}">
       <formula1>"Mohamed, Adel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:F4" xr:uid="{08A2BFBC-CCAB-4301-A523-47B855654D2F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:F4 E6:F6 E8:F8 E10:F10 E12:F12 E14:F14 E16:F16 E18:F18 E20:F20 E22:F22 E24:F24 E26:F27 E29:F30 E32:F33 E35:F36 E38:F39 E41:F42 E44:F45 E47:F48 E50:F51 E53:F54 E56:F58 E60:F62 E64:F65" xr:uid="{08A2BFBC-CCAB-4301-A523-47B855654D2F}">
       <formula1>"Ready to test, Passed, Failed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>